<commit_message>
[F2] Add runnable version
</commit_message>
<xml_diff>
--- a/test-data/F2.xlsx
+++ b/test-data/F2.xlsx
@@ -9,29 +9,23 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="F2-1" sheetId="1" r:id="rId1"/>
+    <sheet name="F2-2" sheetId="2" r:id="rId2"/>
+    <sheet name="F2-3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="42">
   <si>
     <t>ID</t>
   </si>
   <si>
-    <t>File size</t>
-  </si>
-  <si>
     <t>File path</t>
   </si>
   <si>
@@ -41,25 +35,118 @@
     <t>F2-1-1</t>
   </si>
   <si>
+    <t>test.php</t>
+  </si>
+  <si>
+    <t>testing1</t>
+  </si>
+  <si>
+    <t>success</t>
+  </si>
+  <si>
     <t>F2-1-2</t>
   </si>
   <si>
+    <t>aaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaa</t>
+  </si>
+  <si>
     <t>F2-1-3</t>
   </si>
   <si>
+    <t>aaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaa</t>
+  </si>
+  <si>
     <t>F2-1-4</t>
   </si>
   <si>
+    <t>aaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaa</t>
+  </si>
+  <si>
+    <t>fail</t>
+  </si>
+  <si>
     <t>F2-1-5</t>
   </si>
   <si>
+    <t>less.txt</t>
+  </si>
+  <si>
+    <t>testing2</t>
+  </si>
+  <si>
     <t>F2-1-6</t>
   </si>
   <si>
+    <t>equals.txt</t>
+  </si>
+  <si>
+    <t>testing3</t>
+  </si>
+  <si>
     <t>F2-1-7</t>
   </si>
   <si>
-    <t>F2-1-8</t>
+    <t>more.txt</t>
+  </si>
+  <si>
+    <t>testing4</t>
+  </si>
+  <si>
+    <t>F2-2-1</t>
+  </si>
+  <si>
+    <t>F2-2-2</t>
+  </si>
+  <si>
+    <t>F2-2-3</t>
+  </si>
+  <si>
+    <t>F2-2-4</t>
+  </si>
+  <si>
+    <t>Expected status</t>
+  </si>
+  <si>
+    <t>Expected filename on server</t>
+  </si>
+  <si>
+    <t>F2-3-1</t>
+  </si>
+  <si>
+    <t>F2-3-2</t>
+  </si>
+  <si>
+    <t>F2-3-3</t>
+  </si>
+  <si>
+    <t>F2-3-4</t>
+  </si>
+  <si>
+    <t>F2-3-5</t>
+  </si>
+  <si>
+    <t>F2-3-6</t>
+  </si>
+  <si>
+    <t>F2-3-7</t>
+  </si>
+  <si>
+    <t>F2-3-8</t>
+  </si>
+  <si>
+    <t>testing/special1</t>
+  </si>
+  <si>
+    <t>testingspecial1</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>testing/special2</t>
+  </si>
+  <si>
+    <t>hello/aaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaa</t>
   </si>
 </sst>
 </file>
@@ -391,70 +478,433 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="18.109375" customWidth="1"/>
+    <col min="5" max="5" width="25" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="D1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>11</v>
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="15.44140625" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" customWidth="1"/>
+    <col min="5" max="5" width="30.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
[F2] Add filename check for assignment
</commit_message>
<xml_diff>
--- a/test-data/F2.xlsx
+++ b/test-data/F2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
   </bookViews>
   <sheets>
     <sheet name="F2-1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="47">
   <si>
     <t>ID</t>
   </si>
@@ -137,9 +137,6 @@
     <t>testing/special1</t>
   </si>
   <si>
-    <t>testingspecial1</t>
-  </si>
-  <si>
     <t>None</t>
   </si>
   <si>
@@ -147,6 +144,24 @@
   </si>
   <si>
     <t>hello/aaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaa</t>
+  </si>
+  <si>
+    <t>testing1.php</t>
+  </si>
+  <si>
+    <t>testingspecial1.php</t>
+  </si>
+  <si>
+    <t>aaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaa.txt</t>
+  </si>
+  <si>
+    <t>aaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaa.txt</t>
+  </si>
+  <si>
+    <t>testing2.txt</t>
+  </si>
+  <si>
+    <t>testing3.txt</t>
   </si>
 </sst>
 </file>
@@ -480,8 +495,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -521,7 +536,7 @@
         <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>5</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -538,7 +553,7 @@
         <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>8</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -555,7 +570,7 @@
         <v>6</v>
       </c>
       <c r="E4" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -572,7 +587,7 @@
         <v>13</v>
       </c>
       <c r="E5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -589,7 +604,7 @@
         <v>6</v>
       </c>
       <c r="E6" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -606,7 +621,7 @@
         <v>6</v>
       </c>
       <c r="E7" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -623,7 +638,7 @@
         <v>13</v>
       </c>
       <c r="E8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -637,7 +652,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -677,7 +692,7 @@
         <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>5</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -694,7 +709,7 @@
         <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -711,7 +726,7 @@
         <v>13</v>
       </c>
       <c r="E4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -728,7 +743,7 @@
         <v>13</v>
       </c>
       <c r="E5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -740,8 +755,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -782,7 +797,7 @@
         <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>5</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -799,7 +814,7 @@
         <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -816,7 +831,7 @@
         <v>13</v>
       </c>
       <c r="E4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -833,7 +848,7 @@
         <v>13</v>
       </c>
       <c r="E5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -850,7 +865,7 @@
         <v>6</v>
       </c>
       <c r="E6" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -861,13 +876,13 @@
         <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D7" t="s">
         <v>13</v>
       </c>
       <c r="E7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -878,13 +893,13 @@
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D8" t="s">
         <v>13</v>
       </c>
       <c r="E8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -895,13 +910,13 @@
         <v>21</v>
       </c>
       <c r="C9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D9" t="s">
         <v>13</v>
       </c>
       <c r="E9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[F2] Change expected filename in test-data
</commit_message>
<xml_diff>
--- a/test-data/F2.xlsx
+++ b/test-data/F2.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="49">
   <si>
     <t>ID</t>
   </si>
@@ -32,6 +32,12 @@
     <t>Name</t>
   </si>
   <si>
+    <t>Expected status</t>
+  </si>
+  <si>
+    <t>Expected filename on server</t>
+  </si>
+  <si>
     <t>F2-1-1</t>
   </si>
   <si>
@@ -44,12 +50,21 @@
     <t>success</t>
   </si>
   <si>
+    <t>testing1.php</t>
+  </si>
+  <si>
+    <t>Passed</t>
+  </si>
+  <si>
     <t>F2-1-2</t>
   </si>
   <si>
     <t>aaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaa</t>
   </si>
   <si>
+    <t>Failed</t>
+  </si>
+  <si>
     <t>F2-1-3</t>
   </si>
   <si>
@@ -65,6 +80,9 @@
     <t>fail</t>
   </si>
   <si>
+    <t>None</t>
+  </si>
+  <si>
     <t>F2-1-5</t>
   </si>
   <si>
@@ -74,6 +92,9 @@
     <t>testing2</t>
   </si>
   <si>
+    <t>testing2.txt</t>
+  </si>
+  <si>
     <t>F2-1-6</t>
   </si>
   <si>
@@ -83,6 +104,9 @@
     <t>testing3</t>
   </si>
   <si>
+    <t>testing3.txt</t>
+  </si>
+  <si>
     <t>F2-1-7</t>
   </si>
   <si>
@@ -104,12 +128,6 @@
     <t>F2-2-4</t>
   </si>
   <si>
-    <t>Expected status</t>
-  </si>
-  <si>
-    <t>Expected filename on server</t>
-  </si>
-  <si>
     <t>F2-3-1</t>
   </si>
   <si>
@@ -125,43 +143,31 @@
     <t>F2-3-5</t>
   </si>
   <si>
+    <t>testing/special1</t>
+  </si>
+  <si>
+    <t>testingspecial1.php</t>
+  </si>
+  <si>
     <t>F2-3-6</t>
   </si>
   <si>
+    <t>testing/special2</t>
+  </si>
+  <si>
     <t>F2-3-7</t>
   </si>
   <si>
+    <t>hello/aaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaa</t>
+  </si>
+  <si>
     <t>F2-3-8</t>
   </si>
   <si>
-    <t>testing/special1</t>
-  </si>
-  <si>
-    <t>None</t>
-  </si>
-  <si>
-    <t>testing/special2</t>
-  </si>
-  <si>
-    <t>hello/aaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaa</t>
-  </si>
-  <si>
-    <t>testing1.php</t>
-  </si>
-  <si>
-    <t>testingspecial1.php</t>
-  </si>
-  <si>
-    <t>aaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaa.txt</t>
-  </si>
-  <si>
-    <t>aaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaa.txt</t>
-  </si>
-  <si>
-    <t>testing2.txt</t>
-  </si>
-  <si>
-    <t>testing3.txt</t>
+    <t>aaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaa.php</t>
+  </si>
+  <si>
+    <t>aaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaa.php</t>
   </si>
 </sst>
 </file>
@@ -493,10 +499,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -505,7 +511,7 @@
     <col min="5" max="5" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -516,134 +522,155 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" t="s">
         <v>10</v>
-      </c>
-      <c r="D4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
@@ -672,78 +699,78 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>41</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E3" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E4" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E5" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -777,146 +804,146 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>41</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E3" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E4" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E5" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D6" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C7" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="D7" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E7" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="B8" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="D8" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E8" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="D9" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E9" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>